<commit_message>
add: 파일로 MethodExtractor-1.0-SNAPSHOT.jar 에 입력값 전달
</commit_message>
<xml_diff>
--- a/java답안예시01.xlsx
+++ b/java답안예시01.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1747" uniqueCount="588">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1747" uniqueCount="587">
   <si>
     <t>이름</t>
   </si>
@@ -8564,7 +8564,7 @@
 점수: 0</t>
   </si>
   <si>
-    <t>[2번 문제] - 1번 케이스 오답: (유저)"template not found with method info output: Found method 'solution'.\nReturn type: void\nParameters: [int star]" ⊄ (모범결과)["*****\n ***\n  *\n ***\n*****"]</t>
+    <t>[2번 문제] - 1번 케이스 오답: (유저)"채점을 위한 템플릿 코드를 찾지 못했습니다. 제출한 코드의 형식: Found method 'solution'.\nReturn type: void\nParameters: [int star]" ⊄ (모범결과)["*****\n ***\n  *\n ***\n*****"]</t>
   </si>
   <si>
     <t xml:space="preserve">문제: 1번 문제
@@ -8586,8 +8586,10 @@
 점수: 0</t>
   </si>
   <si>
-    <t xml:space="preserve">[2번 문제] - 1번 케이스 오답: (유저)"template not found with method info output: Found method 'solution'.\nReturn type: void\nParameters: [int star]" ⊄ (모범결과)["*****\n ***\n  *\n ***\n*****"]
-[3번 문제] - 1번 케이스 오답: (유저)"Command failed: echo \"import java.util.Arrays;\nimport java.util.Comparator;\nimport java.util.HashMap;\n\npublic class Main {\n    public String[] solution(String[] arr, int n) {\n\n        HashMap&lt;String, String&gt; map = new HashMap&lt;&gt;();\n        HashMap&lt;String, String &gt; duplicatedMap = new HashMap&lt;&gt;();\n        for (String s : arr) {\n            if (map.get(s) == null) {\n                map.put(s, s);\n                System.out.println(\"map.get(s) = \" + map.get(s));\n            } else {\n                duplicatedMap.put(s, s);\n            }\n        }\n        for (String key : duplicatedMap.keySet()) {\n            map.remove(key);\n        }\n\n        // 정답 배열 삽입\n        String[] answer = new String[map.size()];\n        int idx = 0;\n        for (String key : map.keySet()) {\n            answer[idx++] = map.get(key);\n        }\n\n        // 정렬\n        Arrays.sort(answer, new Comparator&lt;String &gt;() {\n            @Override\n            public int compare(String o1, String o2) {\n                if (o1.charAt(n) == o2.charAt(n)) {\n                    return o1.compareTo(o2);\n                }\n                return o1.charAt(n) - o2.charAt(n);\n            }\n        });\n        return answer;\n    }\n\n    public static void main(String[] args) {\n        Main method = new Main();\n        String[] arr = {\"coke\", \"water\", \"glass\", \"dog\", \"dog\", \"yogurt\", \"vitamin\"};\n        int n = 2;\n        System.out.println(Arrays.toString(method.solution(arr, n)));\n    }\n}\n\" | java -jar /Users/gimjeonghyeon/WebstormProjects/auto-score/src/score/language/libs/MethodExtractor-1.0-SNAPSHOT.jar\n/bin/sh: -c: line 12: syntax error near unexpected token `('\n/bin/sh: -c: line 12: `                System.out.println(\"map.get(s) = \" + map.get(s));'\n" ⊄ (모범결과)[["car","bed","sun"]]</t>
+    <t xml:space="preserve">[2번 문제] - 1번 케이스 오답: (유저)"채점을 위한 템플릿 코드를 찾지 못했습니다. 제출한 코드의 형식: Found method 'solution'.\nReturn type: void\nParameters: [int star]" ⊄ (모범결과)["*****\n ***\n  *\n ***\n*****"]
+[3번 문제] - 1번 케이스 오답: (유저)null ⊄ (모범결과)[["car","bed","sun"]]
+[3번 문제] - 2번 케이스 오답: (유저)null ⊄ (모범결과)[["apple","car","cat"]]
+[3번 문제] - 3번 케이스 오답: (유저)null ⊄ (모범결과)[["glass","yogurt","coke","vitamin","water"]]</t>
   </si>
   <si>
     <t xml:space="preserve">문제: 2번 문제
@@ -8596,24 +8598,24 @@
 점수: 66</t>
   </si>
   <si>
-    <t xml:space="preserve">[2번 문제] - 1번 케이스 오답: (유저)"template not found with method info output: Found method 'solution'.\nReturn type: void\nParameters: [int star]" ⊄ (모범결과)["*****\n ***\n  *\n ***\n*****"]
+    <t xml:space="preserve">[2번 문제] - 1번 케이스 오답: (유저)"채점을 위한 템플릿 코드를 찾지 못했습니다. 제출한 코드의 형식: Found method 'solution'.\nReturn type: void\nParameters: [int star]" ⊄ (모범결과)["*****\n ***\n  *\n ***\n*****"]
 [3번 문제] - 2번 케이스 오답: (유저)["apple","cat","car"] ⊄ (모범결과)[["apple","car","cat"]]</t>
   </si>
   <si>
-    <t xml:space="preserve">[2번 문제] - 1번 케이스 오답: (유저)"template not found with method info output: Found method 'solution'.\nReturn type: void\nParameters: [int star]" ⊄ (모범결과)["*****\n ***\n  *\n ***\n*****"]
+    <t xml:space="preserve">[2번 문제] - 1번 케이스 오답: (유저)"채점을 위한 템플릿 코드를 찾지 못했습니다. 제출한 코드의 형식: Found method 'solution'.\nReturn type: void\nParameters: [int star]" ⊄ (모범결과)["*****\n ***\n  *\n ***\n*****"]
 [3번 문제] - 1번 케이스 오답: (유저)["car","bed","brush","sun"] ⊄ (모범결과)[["car","bed","sun"]]
 [3번 문제] - 2번 케이스 오답: (유저)["apple","banana","car","cat"] ⊄ (모범결과)[["apple","car","cat"]]
 [3번 문제] - 3번 케이스 오답: (유저)["glass","dog","yogurt","coke","vitamin","water"] ⊄ (모범결과)[["glass","yogurt","coke","vitamin","water"]]</t>
   </si>
   <si>
-    <t xml:space="preserve">[2번 문제] - 1번 케이스 오답: (유저)"template not found with method info output: Found method 'solution'.\nReturn type: void\nParameters: [int n]" ⊄ (모범결과)["*****\n ***\n  *\n ***\n*****"]
+    <t xml:space="preserve">[2번 문제] - 1번 케이스 오답: (유저)"채점을 위한 템플릿 코드를 찾지 못했습니다. 제출한 코드의 형식: Found method 'solution'.\nReturn type: void\nParameters: [int n]" ⊄ (모범결과)["*****\n ***\n  *\n ***\n*****"]
 [3번 문제] - 1번 케이스 오답: (유저)["car","bed","brush","sun"] ⊄ (모범결과)[["car","bed","sun"]]
 [3번 문제] - 2번 케이스 오답: (유저)["apple","banana","car","cat"] ⊄ (모범결과)[["apple","car","cat"]]
 [3번 문제] - 3번 케이스 오답: (유저)["glass","dog","yogurt","coke","vitamin","water"] ⊄ (모범결과)[["glass","yogurt","coke","vitamin","water"]]</t>
   </si>
   <si>
     <t xml:space="preserve">[1번 문제] - 1번 케이스 오답: (유저)"제출된 userCode 가 없습니다." ⊄ (모범결과)[[[4,6],[7,-9]]]
-[2번 문제] - 1번 케이스 오답: (유저)"template not found with method info output: Found method 'solution'.\nReturn type: void\nParameters: [int star]" ⊄ (모범결과)["*****\n ***\n  *\n ***\n*****"]
+[2번 문제] - 1번 케이스 오답: (유저)"채점을 위한 템플릿 코드를 찾지 못했습니다. 제출한 코드의 형식: Found method 'solution'.\nReturn type: void\nParameters: [int star]" ⊄ (모범결과)["*****\n ***\n  *\n ***\n*****"]
 [3번 문제] - 1번 케이스 오답: (유저)["car","bed","brush","sun"] ⊄ (모범결과)[["car","bed","sun"]]
 [3번 문제] - 2번 케이스 오답: (유저)["apple","banana","car","cat"] ⊄ (모범결과)[["apple","car","cat"]]
 [3번 문제] - 3번 케이스 오답: (유저)["glass","dog","yogurt","coke","vitamin","water"] ⊄ (모범결과)[["glass","yogurt","coke","vitamin","water"]]</t>
@@ -8628,9 +8630,7 @@
 [3번 문제] - 3번 케이스 오답: (유저)["glass","dog","yogurt","coke","vitamin","water"] ⊄ (모범결과)[["glass","yogurt","coke","vitamin","water"]]</t>
   </si>
   <si>
-    <t xml:space="preserve">[3번 문제] - 1번 케이스 오답: (유저)null ⊄ (모범결과)[["car","bed","sun"]]
-[3번 문제] - 2번 케이스 오답: (유저)null ⊄ (모범결과)[["apple","car","cat"]]
-[3번 문제] - 3번 케이스 오답: (유저)null ⊄ (모범결과)[["glass","yogurt","coke","vitamin","water"]]</t>
+    <t/>
   </si>
   <si>
     <t xml:space="preserve">문제: 1번 문제
@@ -8655,27 +8655,23 @@
 [3번 문제] - 1번 케이스 오답: (유저)"Failed to parse the code. Details:\nParse error. Found  \"List\" &lt;IDENTIFIER&gt;, expected one of  \";\" \"@\" \"\\u001a\" \"abstract\" \"class\" \"default\" \"enum\" \"final\" \"import\" \"interface\" \"module\" \"native\" \"open\" \"private\" \"protected\" \"public\" \"record\" \"static\" \"strictfp\" \"synchronized\" \"transient\" \"transitive\" \"volatile\" &lt;EOF&gt;\nProblem stacktrace : \n  com.github.javaparser.GeneratedJavaParser.generateParseException(GeneratedJavaParser.java:13708)\n  com.github.javaparser.GeneratedJavaParser.jj_consume_token(GeneratedJavaParser.java:13554)\n  com.github.javaparser.GeneratedJavaParser.CompilationUnit(GeneratedJavaParser.java:204)\n  com.github.javaparser.JavaParser.parse(JavaParser.java:123)\n  com.mycompany.app.App.main(App.java:36)" ⊄ (모범결과)[["car","bed","sun"]]</t>
   </si>
   <si>
-    <t xml:space="preserve">[2번 문제] - 1번 케이스 오답: (유저)"template not found with method info output: Found method 'solution'.\nReturn type: void\nParameters: [int star]" ⊄ (모범결과)["*****\n ***\n  *\n ***\n*****"]
-[3번 문제] - 1번 케이스 오답: (유저)null ⊄ (모범결과)[["car","bed","sun"]]
-[3번 문제] - 2번 케이스 오답: (유저)null ⊄ (모범결과)[["apple","car","cat"]]
-[3번 문제] - 3번 케이스 오답: (유저)null ⊄ (모범결과)[["glass","yogurt","coke","vitamin","water"]]</t>
-  </si>
-  <si>
     <t xml:space="preserve">문제: 1번 문제
 점수: 0
 문제: 2번 문제
 점수: 0</t>
   </si>
   <si>
-    <t xml:space="preserve">[1번 문제] - 1번 케이스 오답: (유저)"template not found with method info output: Found method 'solution'.\nReturn type: int[][]\nParameters: [int[][] arr1, int[][] arr2, Boolean[][] signs]" ⊄ (모범결과)[[[4,6],[7,-9]]]
-[2번 문제] - 1번 케이스 오답: (유저)"template not found with method info output: Found method 'solution'.\nReturn type: void\nParameters: [int n]" ⊄ (모범결과)["*****\n ***\n  *\n ***\n*****"]</t>
+    <t xml:space="preserve">[1번 문제] - 1번 케이스 오답: (유저)"채점을 위한 템플릿 코드를 찾지 못했습니다. 제출한 코드의 형식: Found method 'solution'.\nReturn type: int[][]\nParameters: [int[][] arr1, int[][] arr2, Boolean[][] signs]" ⊄ (모범결과)[[[4,6],[7,-9]]]
+[2번 문제] - 1번 케이스 오답: (유저)"채점을 위한 템플릿 코드를 찾지 못했습니다. 제출한 코드의 형식: Found method 'solution'.\nReturn type: void\nParameters: [int n]" ⊄ (모범결과)["*****\n ***\n  *\n ***\n*****"]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[3번 문제] - 1번 케이스 오답: (유저)null ⊄ (모범결과)[["car","bed","sun"]]
+[3번 문제] - 2번 케이스 오답: (유저)null ⊄ (모범결과)[["apple","car","cat"]]
+[3번 문제] - 3번 케이스 오답: (유저)null ⊄ (모범결과)[["glass","yogurt","coke","vitamin","water"]]</t>
   </si>
   <si>
     <t xml:space="preserve">[1번 문제] - 1번 케이스 오답: (유저)"Failed to parse the code. Details:\n(line 1,col 5) Parse error. Found \"int\", expected one of  \";\" \"@\" \"class\" \"enum\" \"interface\" \"module\" \"open\" \"record\"\nProblem stacktrace : \n  com.github.javaparser.GeneratedJavaParser.generateParseException(GeneratedJavaParser.java:13708)\n  com.github.javaparser.GeneratedJavaParser.jj_consume_token(GeneratedJavaParser.java:13554)\n  com.github.javaparser.GeneratedJavaParser.CompilationUnit(GeneratedJavaParser.java:182)\n  com.github.javaparser.JavaParser.parse(JavaParser.java:123)\n  com.mycompany.app.App.main(App.java:36)" ⊄ (모범결과)[[[4,6],[7,-9]]]
 [2번 문제] - 1번 케이스 오답: (유저)"Failed to parse the code. Details:\n(line 1,col 5) Parse error. Found \"void\", expected one of  \";\" \"@\" \"class\" \"enum\" \"interface\" \"module\" \"open\" \"record\"\nProblem stacktrace : \n  com.github.javaparser.GeneratedJavaParser.generateParseException(GeneratedJavaParser.java:13708)\n  com.github.javaparser.GeneratedJavaParser.jj_consume_token(GeneratedJavaParser.java:13554)\n  com.github.javaparser.GeneratedJavaParser.CompilationUnit(GeneratedJavaParser.java:182)\n  com.github.javaparser.JavaParser.parse(JavaParser.java:123)\n  com.mycompany.app.App.main(App.java:36)" ⊄ (모범결과)["*****\n ***\n  *\n ***\n*****"]</t>
-  </si>
-  <si>
-    <t/>
   </si>
   <si>
     <t xml:space="preserve">[1번 문제] - 1번 케이스 오답: (유저)[[4,6],[7,-3]] ⊄ (모범결과)[[[4,6],[7,-9]]]
@@ -51622,13 +51618,13 @@
         <v>93</v>
       </c>
       <c r="F20" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G20" t="s">
-        <v>574</v>
+        <v>576</v>
       </c>
       <c r="H20">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I20" t="s">
         <v>576</v>
@@ -51822,7 +51818,7 @@
         <v>1</v>
       </c>
       <c r="I27" t="s">
-        <v>582</v>
+        <v>568</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
@@ -51842,13 +51838,13 @@
         <v>0</v>
       </c>
       <c r="G28" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="H28">
         <v>0</v>
       </c>
       <c r="I28" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
@@ -51897,7 +51893,7 @@
         <v>0</v>
       </c>
       <c r="I30" t="s">
-        <v>576</v>
+        <v>584</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
@@ -51917,7 +51913,7 @@
         <v>0</v>
       </c>
       <c r="G31" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="H31">
         <v>0</v>
@@ -51940,13 +51936,13 @@
         <v>1</v>
       </c>
       <c r="G32" t="s">
-        <v>586</v>
+        <v>576</v>
       </c>
       <c r="H32">
         <v>3</v>
       </c>
       <c r="I32" t="s">
-        <v>586</v>
+        <v>576</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
@@ -52070,13 +52066,13 @@
         <v>0</v>
       </c>
       <c r="G37" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="H37">
         <v>0</v>
       </c>
       <c r="I37" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
@@ -52093,13 +52089,13 @@
         <v>0</v>
       </c>
       <c r="G38" t="s">
-        <v>586</v>
+        <v>576</v>
       </c>
       <c r="H38">
         <v>1</v>
       </c>
       <c r="I38" t="s">
-        <v>586</v>
+        <v>576</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
@@ -52113,13 +52109,13 @@
         <v>0</v>
       </c>
       <c r="G39" t="s">
-        <v>586</v>
+        <v>576</v>
       </c>
       <c r="H39">
         <v>0</v>
       </c>
       <c r="I39" t="s">
-        <v>586</v>
+        <v>576</v>
       </c>
     </row>
   </sheetData>

</xml_diff>